<commit_message>
Update after Dec2019 jolts release
</commit_message>
<xml_diff>
--- a/raw_data/us_initial_claims.xlsx
+++ b/raw_data/us_initial_claims.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Data\RStudio\git\jolts\raw_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89CA72E-6518-46FD-8FE2-C70D8CAE37E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="300" windowWidth="19440" windowHeight="14730"/>
+    <workbookView xWindow="-120" yWindow="300" windowWidth="19440" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="TRNR_6d07f31956b14845a229522d21f31820_1048_1" hidden="1">Planilha1!$A$1</definedName>
+    <definedName name="TRNR_4bd2636e722c4b1e889263c4eb7a7672_1051_1" hidden="1">Planilha1!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Lucas Aguiar de Araujo Pereira</author>
+    <author>Paulo Gustavo Grahl</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3FAE1832-E242-4D43-BDDF-8F78231244B6}">
       <text>
         <r>
           <rPr>
@@ -43,7 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>=DSGRID("USUNCLM"," ","2000-01-01","-0D","W","RowHeader=true;ColHeader=true;Code=true;DispSeriesDescription=false;YearlyTSFormat=false;QuarterlyTSFormat=false","")</t>
         </r>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,7 +88,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,7 +139,7 @@
       <tp t="s">
         <v>Name</v>
         <stp/>
-        <stp>750c63bc-2dce-42fe-beb4-79c5d00b0e1e</stp>
+        <stp>2c27bbea-434d-4f04-aea2-9e0f9cdb25cb</stp>
         <tr r="A1" s="1"/>
       </tp>
     </main>
@@ -430,17 +436,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1049"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1025" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1037" workbookViewId="0">
       <selection activeCell="B1049" sqref="B1049"/>
     </sheetView>
   </sheetViews>
@@ -8806,7 +8812,7 @@
       <c r="A1045" s="1">
         <v>43819</v>
       </c>
-      <c r="B1045">
+      <c r="B1045" s="2">
         <v>224</v>
       </c>
     </row>
@@ -8814,7 +8820,7 @@
       <c r="A1046" s="1">
         <v>43826</v>
       </c>
-      <c r="B1046">
+      <c r="B1046" s="2">
         <v>223</v>
       </c>
     </row>
@@ -8822,7 +8828,7 @@
       <c r="A1047" s="1">
         <v>43833</v>
       </c>
-      <c r="B1047">
+      <c r="B1047" s="2">
         <v>214</v>
       </c>
     </row>
@@ -8830,21 +8836,45 @@
       <c r="A1048" s="1">
         <v>43840</v>
       </c>
-      <c r="B1048">
-        <v>204</v>
+      <c r="B1048" s="2">
+        <v>205</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1049" s="1">
         <v>43847</v>
       </c>
-      <c r="B1049">
-        <v>204</v>
+      <c r="B1049" s="2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1050" s="1">
+        <v>43854</v>
+      </c>
+      <c r="B1050">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1051" s="1">
+        <v>43861</v>
+      </c>
+      <c r="B1051">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1052" s="1">
+        <v>43868</v>
+      </c>
+      <c r="B1052">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="TRAFO" prompt="$A$1:$B$1049" sqref="A1"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="TRAFO" prompt="$A$1:$B$1052" sqref="A1" xr:uid="{9FB94DCC-37B9-4275-B811-7963A894F065}"/>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>